<commit_message>
Extract CourseData From SC file
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSource/SC.xlsx
+++ b/src/main/resources/dataSource/SC.xlsx
@@ -2270,6 +2270,18 @@
   </si>
   <si>
     <t>BAOUCHI</t>
+  </si>
+  <si>
+    <t>Mle1</t>
+  </si>
+  <si>
+    <t>Mle2</t>
+  </si>
+  <si>
+    <t>Mle3</t>
+  </si>
+  <si>
+    <t>Mle4</t>
   </si>
 </sst>
 </file>
@@ -2642,8 +2654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="D1">
+      <selection activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2668,7 +2680,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>752</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -2680,7 +2692,7 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>6</v>
+        <v>753</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
@@ -2692,7 +2704,7 @@
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>6</v>
+        <v>754</v>
       </c>
       <c r="P1" t="s">
         <v>13</v>
@@ -2704,7 +2716,7 @@
         <v>15</v>
       </c>
       <c r="S1" t="s">
-        <v>6</v>
+        <v>755</v>
       </c>
       <c r="T1" t="s">
         <v>16</v>

</xml_diff>